<commit_message>
update README & Finances workbook
</commit_message>
<xml_diff>
--- a/input/Finances.xlsx
+++ b/input/Finances.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="129">
   <si>
     <t>Date</t>
   </si>
@@ -332,6 +332,72 @@
   </si>
   <si>
     <t>California plane ticket</t>
+  </si>
+  <si>
+    <t>Meat Project KBBQ for 2</t>
+  </si>
+  <si>
+    <t>Scale from Amazon</t>
+  </si>
+  <si>
+    <t>Transfer to Fidelity account</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Paycheck (80 hrs)</t>
+  </si>
+  <si>
+    <t>Costco Groceries</t>
+  </si>
+  <si>
+    <t>Quarterly car insurance</t>
+  </si>
+  <si>
+    <t>Cafe onion rings</t>
+  </si>
+  <si>
+    <t>OV Beach Tavern for 2</t>
+  </si>
+  <si>
+    <t>Venmo Jason for food</t>
+  </si>
+  <si>
+    <t>Venmo Jason for Gas</t>
+  </si>
+  <si>
+    <t>A World of Good for 2</t>
+  </si>
+  <si>
+    <t>WikiPedia donation</t>
+  </si>
+  <si>
+    <t>Bday card for Dad</t>
+  </si>
+  <si>
+    <t>Gift</t>
+  </si>
+  <si>
+    <t>Pillow from Kohl's</t>
+  </si>
+  <si>
+    <t>Gift card for Dad</t>
+  </si>
+  <si>
+    <t>Beer from Jimmy's Old Town Tavern</t>
+  </si>
+  <si>
+    <t>Wegmans groceries</t>
+  </si>
+  <si>
+    <t>TeaDo for 3</t>
+  </si>
+  <si>
+    <t>Lunch from cafe</t>
+  </si>
+  <si>
+    <t>Paycheck (78.5 hrs)</t>
   </si>
   <si>
     <t>July</t>
@@ -414,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -512,6 +578,9 @@
     <xf borderId="0" fillId="5" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -9198,9 +9267,15 @@
       <c r="A6" s="34">
         <v>45111.0</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="B6" s="35">
+        <v>-82.89</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="E6" s="37"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
@@ -9225,12 +9300,16 @@
       <c r="Z6" s="37"/>
     </row>
     <row r="7">
-      <c r="A7" s="34">
-        <v>45112.0</v>
-      </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="35">
+        <v>-19.07</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>15</v>
+      </c>
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
@@ -9255,12 +9334,16 @@
       <c r="Z7" s="37"/>
     </row>
     <row r="8">
-      <c r="A8" s="34">
-        <v>45113.0</v>
-      </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="35">
+        <v>-2750.14</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>109</v>
+      </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
@@ -9286,11 +9369,17 @@
     </row>
     <row r="9">
       <c r="A9" s="34">
-        <v>45114.0</v>
-      </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
+        <v>45112.0</v>
+      </c>
+      <c r="B9" s="35">
+        <v>2032.76</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>17</v>
+      </c>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
@@ -9315,12 +9404,16 @@
       <c r="Z9" s="37"/>
     </row>
     <row r="10">
-      <c r="A10" s="34">
-        <v>45115.0</v>
-      </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="39">
+        <v>-45.26</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>30</v>
+      </c>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
@@ -9345,12 +9438,16 @@
       <c r="Z10" s="37"/>
     </row>
     <row r="11">
-      <c r="A11" s="34">
-        <v>45116.0</v>
-      </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="35">
+        <v>-31.48</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="E11" s="37"/>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
@@ -9376,11 +9473,17 @@
     </row>
     <row r="12">
       <c r="A12" s="34">
-        <v>45117.0</v>
-      </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+        <v>45113.0</v>
+      </c>
+      <c r="B12" s="35">
+        <v>-308.88</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="E12" s="37"/>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
@@ -9406,7 +9509,7 @@
     </row>
     <row r="13">
       <c r="A13" s="34">
-        <v>45118.0</v>
+        <v>45114.0</v>
       </c>
       <c r="B13" s="38"/>
       <c r="C13" s="37"/>
@@ -9436,11 +9539,17 @@
     </row>
     <row r="14">
       <c r="A14" s="34">
-        <v>45119.0</v>
-      </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+        <v>45115.0</v>
+      </c>
+      <c r="B14" s="35">
+        <v>-3.71</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="E14" s="37"/>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
@@ -9466,7 +9575,7 @@
     </row>
     <row r="15">
       <c r="A15" s="34">
-        <v>45120.0</v>
+        <v>45116.0</v>
       </c>
       <c r="B15" s="38"/>
       <c r="C15" s="37"/>
@@ -9496,11 +9605,17 @@
     </row>
     <row r="16">
       <c r="A16" s="34">
-        <v>45121.0</v>
-      </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
+        <v>45117.0</v>
+      </c>
+      <c r="B16" s="35">
+        <v>-36.44</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
@@ -9525,12 +9640,16 @@
       <c r="Z16" s="37"/>
     </row>
     <row r="17">
-      <c r="A17" s="34">
-        <v>45122.0</v>
-      </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="35">
+        <v>-13.0</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="E17" s="37"/>
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
@@ -9555,12 +9674,16 @@
       <c r="Z17" s="37"/>
     </row>
     <row r="18">
-      <c r="A18" s="34">
-        <v>45123.0</v>
-      </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="35">
+        <v>-40.0</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>104</v>
+      </c>
       <c r="E18" s="37"/>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
@@ -9586,11 +9709,17 @@
     </row>
     <row r="19">
       <c r="A19" s="34">
-        <v>45124.0</v>
-      </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
+        <v>45118.0</v>
+      </c>
+      <c r="B19" s="35">
+        <v>-36.96</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="E19" s="37"/>
       <c r="F19" s="37"/>
       <c r="G19" s="37"/>
@@ -9616,11 +9745,17 @@
     </row>
     <row r="20">
       <c r="A20" s="34">
-        <v>45125.0</v>
-      </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
+        <v>45119.0</v>
+      </c>
+      <c r="B20" s="35">
+        <v>-3.1</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>15</v>
+      </c>
       <c r="E20" s="37"/>
       <c r="F20" s="37"/>
       <c r="G20" s="37"/>
@@ -9646,7 +9781,7 @@
     </row>
     <row r="21">
       <c r="A21" s="34">
-        <v>45126.0</v>
+        <v>45120.0</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="37"/>
@@ -9676,11 +9811,17 @@
     </row>
     <row r="22">
       <c r="A22" s="34">
-        <v>45127.0</v>
-      </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
+        <v>45121.0</v>
+      </c>
+      <c r="B22" s="35">
+        <v>-3.71</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="E22" s="37"/>
       <c r="F22" s="37"/>
       <c r="G22" s="37"/>
@@ -9705,12 +9846,16 @@
       <c r="Z22" s="37"/>
     </row>
     <row r="23">
-      <c r="A23" s="34">
-        <v>45128.0</v>
-      </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35">
+        <v>-40.76</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>30</v>
+      </c>
       <c r="E23" s="37"/>
       <c r="F23" s="37"/>
       <c r="G23" s="37"/>
@@ -9735,12 +9880,16 @@
       <c r="Z23" s="37"/>
     </row>
     <row r="24">
-      <c r="A24" s="34">
-        <v>45129.0</v>
-      </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="35">
+        <v>-24.34</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
       <c r="G24" s="37"/>
@@ -9765,12 +9914,16 @@
       <c r="Z24" s="37"/>
     </row>
     <row r="25">
-      <c r="A25" s="34">
-        <v>45130.0</v>
-      </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="35">
+        <v>-5.29</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>120</v>
+      </c>
       <c r="E25" s="37"/>
       <c r="F25" s="37"/>
       <c r="G25" s="37"/>
@@ -9795,12 +9948,16 @@
       <c r="Z25" s="37"/>
     </row>
     <row r="26">
-      <c r="A26" s="34">
-        <v>45131.0</v>
-      </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="35">
+        <v>-27.55</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>15</v>
+      </c>
       <c r="E26" s="37"/>
       <c r="F26" s="37"/>
       <c r="G26" s="37"/>
@@ -9825,12 +9982,16 @@
       <c r="Z26" s="37"/>
     </row>
     <row r="27">
-      <c r="A27" s="34">
-        <v>45132.0</v>
-      </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="35">
+        <v>-40.0</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>120</v>
+      </c>
       <c r="E27" s="37"/>
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
@@ -9856,7 +10017,7 @@
     </row>
     <row r="28">
       <c r="A28" s="34">
-        <v>45133.0</v>
+        <v>45122.0</v>
       </c>
       <c r="B28" s="38"/>
       <c r="C28" s="37"/>
@@ -9886,11 +10047,17 @@
     </row>
     <row r="29">
       <c r="A29" s="34">
-        <v>45134.0</v>
-      </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
+        <v>45123.0</v>
+      </c>
+      <c r="B29" s="35">
+        <v>-32.0</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>66</v>
+      </c>
       <c r="E29" s="37"/>
       <c r="F29" s="37"/>
       <c r="G29" s="37"/>
@@ -9915,12 +10082,16 @@
       <c r="Z29" s="37"/>
     </row>
     <row r="30">
-      <c r="A30" s="34">
-        <v>45135.0</v>
-      </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="35">
+        <v>-8.76</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="E30" s="37"/>
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
@@ -9945,12 +10116,16 @@
       <c r="Z30" s="37"/>
     </row>
     <row r="31">
-      <c r="A31" s="34">
-        <v>45136.0</v>
-      </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="35">
+        <v>-10.33</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>6</v>
+      </c>
       <c r="E31" s="37"/>
       <c r="F31" s="37"/>
       <c r="G31" s="37"/>
@@ -9976,9 +10151,11 @@
     </row>
     <row r="32">
       <c r="A32" s="34">
-        <v>45137.0</v>
-      </c>
-      <c r="B32" s="38"/>
+        <v>45124.0</v>
+      </c>
+      <c r="B32" s="35">
+        <v>-41.25</v>
+      </c>
       <c r="C32" s="37"/>
       <c r="D32" s="37"/>
       <c r="E32" s="37"/>
@@ -10006,11 +10183,17 @@
     </row>
     <row r="33">
       <c r="A33" s="34">
-        <v>45138.0</v>
-      </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
+        <v>45125.0</v>
+      </c>
+      <c r="B33" s="35">
+        <v>-15.9</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="E33" s="37"/>
       <c r="F33" s="37"/>
       <c r="G33" s="37"/>
@@ -10035,15 +10218,18 @@
       <c r="Z33" s="37"/>
     </row>
     <row r="34">
-      <c r="A34" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" s="38">
-        <f>SUM(B2:B33)</f>
-        <v>-549.43</v>
-      </c>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
+      <c r="A34" s="34">
+        <v>45126.0</v>
+      </c>
+      <c r="B34" s="35">
+        <v>-14.58</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="E34" s="37"/>
       <c r="F34" s="37"/>
       <c r="G34" s="37"/>
@@ -10067,6 +10253,433 @@
       <c r="Y34" s="37"/>
       <c r="Z34" s="37"/>
     </row>
+    <row r="35">
+      <c r="A35" s="34"/>
+      <c r="B35" s="35">
+        <v>2000.79</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="37"/>
+      <c r="P35" s="37"/>
+      <c r="Q35" s="37"/>
+      <c r="R35" s="37"/>
+      <c r="S35" s="37"/>
+      <c r="T35" s="37"/>
+      <c r="U35" s="37"/>
+      <c r="V35" s="37"/>
+      <c r="W35" s="37"/>
+      <c r="X35" s="37"/>
+      <c r="Y35" s="37"/>
+      <c r="Z35" s="37"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="34">
+        <v>45127.0</v>
+      </c>
+      <c r="B36" s="38"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="37"/>
+      <c r="O36" s="37"/>
+      <c r="P36" s="37"/>
+      <c r="Q36" s="37"/>
+      <c r="R36" s="37"/>
+      <c r="S36" s="37"/>
+      <c r="T36" s="37"/>
+      <c r="U36" s="37"/>
+      <c r="V36" s="37"/>
+      <c r="W36" s="37"/>
+      <c r="X36" s="37"/>
+      <c r="Y36" s="37"/>
+      <c r="Z36" s="37"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="34">
+        <v>45128.0</v>
+      </c>
+      <c r="B37" s="38"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="37"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="37"/>
+      <c r="W37" s="37"/>
+      <c r="X37" s="37"/>
+      <c r="Y37" s="37"/>
+      <c r="Z37" s="37"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="34">
+        <v>45129.0</v>
+      </c>
+      <c r="B38" s="38"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="37"/>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37"/>
+      <c r="Q38" s="37"/>
+      <c r="R38" s="37"/>
+      <c r="S38" s="37"/>
+      <c r="T38" s="37"/>
+      <c r="U38" s="37"/>
+      <c r="V38" s="37"/>
+      <c r="W38" s="37"/>
+      <c r="X38" s="37"/>
+      <c r="Y38" s="37"/>
+      <c r="Z38" s="37"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="34">
+        <v>45130.0</v>
+      </c>
+      <c r="B39" s="38"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
+      <c r="R39" s="37"/>
+      <c r="S39" s="37"/>
+      <c r="T39" s="37"/>
+      <c r="U39" s="37"/>
+      <c r="V39" s="37"/>
+      <c r="W39" s="37"/>
+      <c r="X39" s="37"/>
+      <c r="Y39" s="37"/>
+      <c r="Z39" s="37"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="34">
+        <v>45131.0</v>
+      </c>
+      <c r="B40" s="38"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="37"/>
+      <c r="N40" s="37"/>
+      <c r="O40" s="37"/>
+      <c r="P40" s="37"/>
+      <c r="Q40" s="37"/>
+      <c r="R40" s="37"/>
+      <c r="S40" s="37"/>
+      <c r="T40" s="37"/>
+      <c r="U40" s="37"/>
+      <c r="V40" s="37"/>
+      <c r="W40" s="37"/>
+      <c r="X40" s="37"/>
+      <c r="Y40" s="37"/>
+      <c r="Z40" s="37"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="34">
+        <v>45132.0</v>
+      </c>
+      <c r="B41" s="38"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="37"/>
+      <c r="O41" s="37"/>
+      <c r="P41" s="37"/>
+      <c r="Q41" s="37"/>
+      <c r="R41" s="37"/>
+      <c r="S41" s="37"/>
+      <c r="T41" s="37"/>
+      <c r="U41" s="37"/>
+      <c r="V41" s="37"/>
+      <c r="W41" s="37"/>
+      <c r="X41" s="37"/>
+      <c r="Y41" s="37"/>
+      <c r="Z41" s="37"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="34">
+        <v>45133.0</v>
+      </c>
+      <c r="B42" s="38"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
+      <c r="O42" s="37"/>
+      <c r="P42" s="37"/>
+      <c r="Q42" s="37"/>
+      <c r="R42" s="37"/>
+      <c r="S42" s="37"/>
+      <c r="T42" s="37"/>
+      <c r="U42" s="37"/>
+      <c r="V42" s="37"/>
+      <c r="W42" s="37"/>
+      <c r="X42" s="37"/>
+      <c r="Y42" s="37"/>
+      <c r="Z42" s="37"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="34">
+        <v>45134.0</v>
+      </c>
+      <c r="B43" s="38"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="37"/>
+      <c r="L43" s="37"/>
+      <c r="M43" s="37"/>
+      <c r="N43" s="37"/>
+      <c r="O43" s="37"/>
+      <c r="P43" s="37"/>
+      <c r="Q43" s="37"/>
+      <c r="R43" s="37"/>
+      <c r="S43" s="37"/>
+      <c r="T43" s="37"/>
+      <c r="U43" s="37"/>
+      <c r="V43" s="37"/>
+      <c r="W43" s="37"/>
+      <c r="X43" s="37"/>
+      <c r="Y43" s="37"/>
+      <c r="Z43" s="37"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="34">
+        <v>45135.0</v>
+      </c>
+      <c r="B44" s="38"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="37"/>
+      <c r="N44" s="37"/>
+      <c r="O44" s="37"/>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="37"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="37"/>
+      <c r="U44" s="37"/>
+      <c r="V44" s="37"/>
+      <c r="W44" s="37"/>
+      <c r="X44" s="37"/>
+      <c r="Y44" s="37"/>
+      <c r="Z44" s="37"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="34">
+        <v>45136.0</v>
+      </c>
+      <c r="B45" s="38"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
+      <c r="O45" s="37"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="37"/>
+      <c r="V45" s="37"/>
+      <c r="W45" s="37"/>
+      <c r="X45" s="37"/>
+      <c r="Y45" s="37"/>
+      <c r="Z45" s="37"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="34">
+        <v>45137.0</v>
+      </c>
+      <c r="B46" s="38"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="37"/>
+      <c r="O46" s="37"/>
+      <c r="P46" s="37"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
+      <c r="T46" s="37"/>
+      <c r="U46" s="37"/>
+      <c r="V46" s="37"/>
+      <c r="W46" s="37"/>
+      <c r="X46" s="37"/>
+      <c r="Y46" s="37"/>
+      <c r="Z46" s="37"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="34">
+        <v>45138.0</v>
+      </c>
+      <c r="B47" s="38"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
+      <c r="M47" s="37"/>
+      <c r="N47" s="37"/>
+      <c r="O47" s="37"/>
+      <c r="P47" s="37"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="37"/>
+      <c r="S47" s="37"/>
+      <c r="T47" s="37"/>
+      <c r="U47" s="37"/>
+      <c r="V47" s="37"/>
+      <c r="W47" s="37"/>
+      <c r="X47" s="37"/>
+      <c r="Y47" s="37"/>
+      <c r="Z47" s="37"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="38">
+        <f>SUM(B2:B47)</f>
+        <v>-151.28</v>
+      </c>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
+      <c r="O48" s="37"/>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="37"/>
+      <c r="T48" s="37"/>
+      <c r="U48" s="37"/>
+      <c r="V48" s="37"/>
+      <c r="W48" s="37"/>
+      <c r="X48" s="37"/>
+      <c r="Y48" s="37"/>
+      <c r="Z48" s="37"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>